<commit_message>
Update Linear Regression Predict Sales Start File.xlsx
</commit_message>
<xml_diff>
--- a/regression/Linear Regression Predict Sales Start File.xlsx
+++ b/regression/Linear Regression Predict Sales Start File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__DSM_LMS_Courses\5_4_Predictive_Supervised\L0 Intuition with Excel\1_Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\apps\UNEXT_PythonDashboard_Streamlit\regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4D6D7C-ED93-4FDD-9A97-111DA19108E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5594E3BC-81F0-44AB-8EBF-230917259964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{23917D7D-B777-4EA8-A31B-9A2D868B7DDC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23917D7D-B777-4EA8-A31B-9A2D868B7DDC}"/>
   </bookViews>
   <sheets>
     <sheet name="UserInterface" sheetId="9" r:id="rId1"/>
@@ -1314,9 +1314,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="12" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1327,6 +1324,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="12" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="60% - Accent4" xfId="3" builtinId="44"/>
@@ -6688,7 +6688,7 @@
         <xdr:cNvPr id="2" name="Picture 1" descr="Logistic Regression in Machine Learning">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6754,7 +6754,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6797,7 +6797,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6842,7 +6842,7 @@
             <xdr:cNvPr id="2" name="Picture 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6850,7 +6850,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Regression_LSq!$B$1:$E$2" spid="_x0000_s6293"/>
+                  <a14:cameraTool cellRange="Regression_LSq!$B$1:$E$2" spid="_x0000_s6295"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -6906,7 +6906,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6947,7 +6947,7 @@
                   <a14:compatExt spid="_x0000_s6209"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000041180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000041180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7289,8 +7289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B503D587-8D7E-450F-A4C0-A10F3D06F133}">
   <dimension ref="B4:F11"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -7304,12 +7304,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="40" t="s">
         <v>237</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
     </row>
     <row r="5" spans="2:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -7333,53 +7333,53 @@
     </row>
     <row r="8" spans="2:6" collapsed="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>243</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="36" t="s">
         <v>224</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="38" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="40">
+      <c r="B10" s="39">
         <f>SUM(C10:E10)</f>
         <v>180</v>
       </c>
-      <c r="C10" s="40">
+      <c r="C10" s="39">
         <v>80</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="39">
         <v>50</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="39">
         <v>50</v>
       </c>
-      <c r="F10" s="40"/>
+      <c r="F10" s="39"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="40">
+      <c r="B11" s="39">
         <f>SUM(C11:E11)</f>
         <v>160</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="39">
         <v>20</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="39">
         <v>80</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="39">
         <v>60</v>
       </c>
-      <c r="F11" s="40"/>
+      <c r="F11" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -23397,7 +23397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736FF200-99B5-4F2D-8734-71DECD8A5778}">
   <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>